<commit_message>
chicken import with breeding pari
</commit_message>
<xml_diff>
--- a/ilri_ges/static/excel/chickens_template.xlsx
+++ b/ilri_ges/static/excel/chickens_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t xml:space="preserve">House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hatch Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Yolk</t>
   </si>
 </sst>
 </file>
@@ -41,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -69,6 +78,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,12 +128,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -139,13 +158,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.71"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -159,6 +182,15 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>